<commit_message>
completion of synching up USP and main branch.
</commit_message>
<xml_diff>
--- a/ExcelTools/Test_Files/manual test2.xlsx
+++ b/ExcelTools/Test_Files/manual test2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ncats_source\Excel\CSharpTest2\Test_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544B060-8A1F-4015-919F-A781056CBC97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C17807-CEE9-4C39-8B57-64003E98730E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="1164">
   <si>
     <t>METHANDRIOL</t>
   </si>
@@ -3504,6 +3504,27 @@
   </si>
   <si>
     <t xml:space="preserve">ISTIRATUMAB </t>
+  </si>
+  <si>
+    <t>STEARIC ACID</t>
+  </si>
+  <si>
+    <t>ANISE OIL</t>
+  </si>
+  <si>
+    <t>PENTAGALLOYLGLUCOSE</t>
+  </si>
+  <si>
+    <t>PETASIN</t>
+  </si>
+  <si>
+    <t>ESCIN</t>
+  </si>
+  <si>
+    <t>CHAMOMILE</t>
+  </si>
+  <si>
+    <t>BENZOIC ACID</t>
   </si>
 </sst>
 </file>
@@ -4810,10 +4831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B14"/>
+  <dimension ref="B2:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4879,6 +4900,41 @@
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>1156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>1163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>